<commit_message>
Regular Expressions - changes added to PayslipProb
</commit_message>
<xml_diff>
--- a/Goals.xlsx
+++ b/Goals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Linda.Johnstone/Documents/fma/c-sharp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD7A4D12-4792-7646-A5FD-9DD0316A830B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0248A7-E5DF-D248-987A-355646AEF584}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7800" yWindow="1740" windowWidth="28040" windowHeight="17440" xr2:uid="{B2AD85C7-1A4B-9248-9590-754E404CCF9B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -95,15 +95,6 @@
     <t>Culture Day 4</t>
   </si>
   <si>
-    <t>Refactor Person.cs so it can be tested. Use same interface</t>
-  </si>
-  <si>
-    <t>Test Person.cs input</t>
-  </si>
-  <si>
-    <t>Regular expressions - use to test Person.cs</t>
-  </si>
-  <si>
     <t>Access modifiers - small projects</t>
   </si>
   <si>
@@ -122,43 +113,35 @@
     <t>Exceptions</t>
   </si>
   <si>
-    <t>New project to be used to continue testing, composition, etc</t>
-  </si>
-  <si>
     <t>Setup pair programming sessions within cohort</t>
+  </si>
+  <si>
+    <t>Refactor Person.cs so that it can be tested NB need to add new PersonInput.cs file as Person.cs only seems to get input and then print it</t>
+  </si>
+  <si>
+    <t>Test Person class to create PersonInput.cs</t>
+  </si>
+  <si>
+    <t>Use Payslip interface to refactor code in Person class</t>
+  </si>
+  <si>
+    <t>Use regular expressions in PersonInput class (testing)</t>
+  </si>
+  <si>
+    <t>New project / kata to understand concepts</t>
+  </si>
+  <si>
+    <t>Do I set up a new repo or tidy up the existing one?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="16"/>
-      <color rgb="FF0066CC"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,12 +155,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FF0066CC"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
       <u/>
       <sz val="16"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -199,24 +197,27 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -533,22 +534,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A68076-8855-474D-BE05-22F022BA6A14}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.83203125" style="3" customWidth="1"/>
-    <col min="3" max="4" width="15.83203125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="15.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="50.83203125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="15.83203125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="66">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,290 +563,306 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="88" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="2" spans="1:4" ht="88">
+      <c r="A2" s="3">
         <v>44060</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2">
-        <v>44064</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" s="3">
+        <v>44064</v>
+      </c>
+      <c r="D2" s="3">
         <v>44060</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="44" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    <row r="3" spans="1:4" ht="44">
+      <c r="A3" s="3">
         <v>44060</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2">
-        <v>44064</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="3">
+        <v>44064</v>
+      </c>
+      <c r="D3" s="3">
         <v>44061</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="44" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="4" spans="1:4" ht="44">
+      <c r="A4" s="3">
         <v>44060</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2">
-        <v>44064</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="3">
+        <v>44064</v>
+      </c>
+      <c r="D4" s="3">
         <v>44061</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="44" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="5" spans="1:4" ht="44">
+      <c r="A5" s="3">
         <v>44060</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2">
-        <v>44064</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="3">
+        <v>44064</v>
+      </c>
+      <c r="D5" s="3">
         <v>44061</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="44" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+    <row r="6" spans="1:4" ht="44">
+      <c r="A6" s="3">
         <v>44060</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2">
-        <v>44064</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="3">
+        <v>44064</v>
+      </c>
+      <c r="D6" s="3">
         <v>44061</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+    <row r="7" spans="1:4" ht="22">
+      <c r="A7" s="3">
         <v>44060</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>44061</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>44061</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="44" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+    <row r="8" spans="1:4" ht="44">
+      <c r="A8" s="3">
         <v>44060</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2">
-        <v>44064</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="C8" s="3">
+        <v>44064</v>
+      </c>
+      <c r="D8" s="3">
         <v>44061</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+    <row r="9" spans="1:4" ht="22">
+      <c r="A9" s="3">
         <v>44061</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>44062</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="3">
         <v>44062</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+    <row r="10" spans="1:4" ht="22">
+      <c r="A10" s="3">
         <v>44063</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>44063</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="3">
         <v>44063</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+    <row r="11" spans="1:4" ht="22">
+      <c r="A11" s="3">
         <v>44060</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>44068</v>
       </c>
-      <c r="D11" s="2">
-        <v>44067</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>44064</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="2">
-        <v>44067</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>44064</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="D11" s="3">
+        <v>44067</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="22">
+      <c r="A12" s="3">
+        <v>44064</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3">
+        <v>44067</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="22">
+      <c r="A13" s="3">
+        <v>44064</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="3">
+        <v>44067</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="22">
+      <c r="A14" s="3">
+        <v>44067</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="3">
+        <v>44067</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="44">
+      <c r="A15" s="3">
+        <v>44067</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="2">
-        <v>44067</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="22" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>44067</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="2">
-        <v>44067</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="44" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>44067</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="2">
-        <v>44067</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="44" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="D15" s="3">
+        <v>44067</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="44">
+      <c r="A16" s="3">
         <v>44063</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="44" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>44064</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="22" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>44064</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="22" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>44064</v>
-      </c>
-      <c r="B19" s="3" t="s">
+    <row r="17" spans="1:3" ht="88">
+      <c r="A17" s="3">
+        <v>44064</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="22">
+      <c r="A18" s="3">
+        <v>44064</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="44">
+      <c r="A19" s="3">
+        <v>44064</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="22">
+      <c r="A20" s="3">
+        <v>44064</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="22" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>44064</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="22">
+      <c r="A21" s="3">
+        <v>44067</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="3" t="s">
+    </row>
+    <row r="22" spans="1:3" ht="22">
+      <c r="A22" s="3">
+        <v>44067</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="44">
+      <c r="A23" s="3">
+        <v>44067</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="22" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+    <row r="24" spans="1:3" ht="44">
+      <c r="A24" s="3">
+        <v>44067</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="22">
+      <c r="A25" s="3">
         <v>44070</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="22" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+    <row r="26" spans="1:3" ht="22">
+      <c r="A26" s="3">
         <v>44077</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="22" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+    <row r="27" spans="1:3" ht="22">
+      <c r="A27" s="3">
         <v>44083</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="22" x14ac:dyDescent="0.2">
-      <c r="B24" s="3" t="s">
+    <row r="28" spans="1:3" ht="22">
+      <c r="B28" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="22" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
-        <v>44067</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="44" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
-        <v>44067</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="44" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
-        <v>44067</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>30</v>
+    <row r="29" spans="1:3" ht="44">
+      <c r="A29" s="3">
+        <v>44067</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D24">
-    <sortCondition ref="D2:D24"/>
-    <sortCondition ref="A2:A24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D28">
+    <sortCondition ref="D2:D28"/>
+    <sortCondition ref="A2:A28"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B15" r:id="rId1" xr:uid="{7A767A50-14C0-A44E-9EA1-AA96ACA9384D}"/>

</xml_diff>